<commit_message>
Minor modifications to conform to new test-file requirements
</commit_message>
<xml_diff>
--- a/test-files/gene-name-modifications/duplicate-gene-top-output.xlsx
+++ b/test-files/gene-name-modifications/duplicate-gene-top-output.xlsx
@@ -19,33 +19,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>rows genes affected/cols genes controlling</t>
   </si>
   <si>
-    <t>duplicate</t>
+    <t>a</t>
   </si>
   <si>
-    <t>A</t>
+    <t>c</t>
   </si>
   <si>
-    <t>B</t>
+    <t>d</t>
   </si>
   <si>
-    <t>C</t>
+    <t>e</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -414,95 +405,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-0.17566519889880799</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>-0.17566519889880838</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>4</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -511,7 +481,7 @@
         <v>9.7143193603914768E-2</v>
       </c>
       <c r="D4">
-        <v>9.7143193603914768E-2</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -519,16 +489,10 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -545,16 +509,10 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -569,64 +527,6 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>-0.38230713137630445</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
         <v>0</v>
       </c>
     </row>

</xml_diff>